<commit_message>
New South Creek data
</commit_message>
<xml_diff>
--- a/matlab/Data_Import/Conversions_v2.xlsx
+++ b/matlab/Data_Import/Conversions_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Hawkesbury\matlab\Data_Import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3952309A-38CD-4651-BC4F-9E07C2DB815F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16248FAA-535E-48B2-B568-2D49B4923121}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
   <si>
     <t>Sal_gperL</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>uS/cm</t>
+  </si>
+  <si>
+    <t>Conductivity</t>
   </si>
 </sst>
 </file>
@@ -542,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="H1" sqref="H1:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,6 +877,20 @@
         <v>11</v>
       </c>
     </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>